<commit_message>
Fix breakdown template import error
</commit_message>
<xml_diff>
--- a/public/files/templates/breakdown-templates.xlsx
+++ b/public/files/templates/breakdown-templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/apps/cost-control/public/files/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Standard Activity</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Equation $v</t>
+  </si>
+  <si>
+    <t>Labour Count</t>
+  </si>
+  <si>
+    <t>Productivity Ref</t>
   </si>
 </sst>
 </file>
@@ -134,15 +140,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="WBS" displayName="WBS" ref="A1:G48" headerRowDxfId="0">
-  <autoFilter ref="A1:G48"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="WBS" displayName="WBS" ref="A1:I48" headerRowDxfId="0">
+  <autoFilter ref="A1:I48"/>
+  <tableColumns count="9">
     <tableColumn id="8" name="Std Code"/>
     <tableColumn id="1" name="Standard Activity" totalsRowLabel="Total"/>
     <tableColumn id="9" name="Breakdown template name"/>
     <tableColumn id="2" name="Resource Code"/>
     <tableColumn id="3" name="Resource Name"/>
     <tableColumn id="4" name="Equation $v"/>
+    <tableColumn id="7" name="Labour Count"/>
+    <tableColumn id="6" name="Productivity Ref"/>
     <tableColumn id="5" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -412,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,12 +433,12 @@
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="25.83203125" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="6" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -450,13 +458,19 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
     </row>
   </sheetData>

</xml_diff>